<commit_message>
Improved formatting and added sheet to html library
</commit_message>
<xml_diff>
--- a/cw.xlsx
+++ b/cw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndy15\Documents\Personal\CWTeams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndy15\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE23101-060D-41F1-AD2E-CD5B0E9078C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A46D65-038B-430F-8AFD-F6EC68B37700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{4D2EA23C-A82B-414D-844B-2B51042E71A8}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,11 +1078,11 @@
         <v>57</v>
       </c>
       <c r="B2" s="32">
-        <f t="shared" ref="B2:B20" si="0">0.6*D2+0.25*E2+0.15*F2</f>
+        <f>0.6*D2+0.25*E2+0.15*F2</f>
         <v>9.9250000000000007</v>
       </c>
       <c r="C2" s="35">
-        <f t="shared" ref="C2:C20" si="1">0.5*D2+0.45*E2+0.05*F2</f>
+        <f>0.5*D2+0.45*E2+0.05*F2</f>
         <v>9.9749999999999996</v>
       </c>
       <c r="D2" s="3">
@@ -1099,29 +1099,29 @@
       </c>
       <c r="H2" s="50">
         <f>SUMIF(G:G, "b", B:B)</f>
-        <v>24.430000000000003</v>
+        <v>9.9250000000000007</v>
       </c>
       <c r="I2" s="51">
         <f>SUMIF(G:G, "b", D:D)/3</f>
-        <v>8.2666666666666675</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="J2" s="51">
         <f>SUMIF(G:G, "b", E:E)/3</f>
-        <v>7.833333333333333</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="K2" s="52">
         <f>SUMIF(G:G, "b", F:F)/3</f>
-        <v>8.1666666666666661</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>48</v>
       </c>
       <c r="M2" s="23">
-        <f t="shared" ref="M2:M41" si="2">0.2*P2+0.8*Q2</f>
+        <f>0.2*P2+0.8*Q2</f>
         <v>9.4</v>
       </c>
       <c r="N2" s="23">
-        <f t="shared" ref="N2:N41" si="3">0.5*Q2+0.3*P2+0.2*O2</f>
+        <f>0.5*Q2+0.3*P2+0.2*O2</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="O2" s="24">
@@ -1139,11 +1139,11 @@
         <v>59</v>
       </c>
       <c r="B3" s="30">
-        <f t="shared" si="0"/>
+        <f>0.6*D3+0.25*E3+0.15*F3</f>
         <v>9.4599999999999991</v>
       </c>
       <c r="C3" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D3+0.45*E3+0.05*F3</f>
         <v>9.48</v>
       </c>
       <c r="D3" s="4">
@@ -1160,29 +1160,29 @@
       </c>
       <c r="H3" s="47">
         <f>SUMIF(G:G, "r", B:B)</f>
-        <v>15.645</v>
+        <v>9.4599999999999991</v>
       </c>
       <c r="I3" s="53">
         <f>SUMIF(G:G, "r", D:D)/3</f>
-        <v>5.3666666666666671</v>
+        <v>3.1999999999999997</v>
       </c>
       <c r="J3" s="53">
         <f>SUMIF(G:G, "r", E:E)/3</f>
-        <v>4.8999999999999995</v>
+        <v>3.1333333333333333</v>
       </c>
       <c r="K3" s="40">
         <f>SUMIF(G:G, "r", F:F)/3</f>
-        <v>5.1333333333333337</v>
+        <v>3</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="M3" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P3+0.8*Q3</f>
         <v>9.1999999999999993</v>
       </c>
       <c r="N3" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q3+0.3*P3+0.2*O3</f>
         <v>8.6999999999999993</v>
       </c>
       <c r="O3" s="17">
@@ -1200,11 +1200,11 @@
         <v>58</v>
       </c>
       <c r="B4" s="31">
-        <f t="shared" si="0"/>
+        <f>0.6*D4+0.25*E4+0.15*F4</f>
         <v>8.7550000000000008</v>
       </c>
       <c r="C4" s="34">
-        <f t="shared" si="1"/>
+        <f>0.5*D4+0.45*E4+0.05*F4</f>
         <v>8.6649999999999991</v>
       </c>
       <c r="D4" s="5">
@@ -1221,29 +1221,29 @@
       </c>
       <c r="H4" s="54">
         <f>SUMIF(G:G, "y", B:B)</f>
-        <v>16.625</v>
+        <v>8.7550000000000008</v>
       </c>
       <c r="I4" s="55">
         <f>SUMIF(G:G, "y", D:D)/3</f>
-        <v>5.7333333333333334</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="J4" s="55">
         <f>SUMIF(G:G, "y", E:E)/3</f>
-        <v>5.3666666666666671</v>
+        <v>2.6333333333333333</v>
       </c>
       <c r="K4" s="56">
         <f>SUMIF(G:G, "y", F:F)/3</f>
-        <v>5.0666666666666664</v>
+        <v>2.4</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="M4" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P4+0.8*Q4</f>
         <v>9.1999999999999993</v>
       </c>
       <c r="N4" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q4+0.3*P4+0.2*O4</f>
         <v>8.1</v>
       </c>
       <c r="O4" s="17">
@@ -1261,11 +1261,11 @@
         <v>65</v>
       </c>
       <c r="B5" s="32">
-        <f t="shared" si="0"/>
+        <f>0.6*D5+0.25*E5+0.15*F5</f>
         <v>8.33</v>
       </c>
       <c r="C5" s="35">
-        <f t="shared" si="1"/>
+        <f>0.5*D5+0.45*E5+0.05*F5</f>
         <v>8.2099999999999991</v>
       </c>
       <c r="D5" s="3">
@@ -1282,29 +1282,29 @@
       </c>
       <c r="H5" s="57">
         <f>SUMIF(G:G, "g", B:B)</f>
-        <v>16.09</v>
+        <v>8.33</v>
       </c>
       <c r="I5" s="58">
         <f>SUMIF(G:G, "g", D:D)/3</f>
-        <v>5.666666666666667</v>
+        <v>2.9</v>
       </c>
       <c r="J5" s="58">
         <f>SUMIF(G:G, "g", E:E)/3</f>
-        <v>4.833333333333333</v>
+        <v>2.5666666666666669</v>
       </c>
       <c r="K5" s="42">
         <f>SUMIF(G:G, "g", F:F)/3</f>
-        <v>5.0333333333333341</v>
+        <v>2.6333333333333333</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="M5" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P5+0.8*Q5</f>
         <v>9.1999999999999993</v>
       </c>
       <c r="N5" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q5+0.3*P5+0.2*O5</f>
         <v>8.1</v>
       </c>
       <c r="O5" s="17">
@@ -1322,11 +1322,11 @@
         <v>61</v>
       </c>
       <c r="B6" s="30">
-        <f t="shared" si="0"/>
+        <f>0.6*D6+0.25*E6+0.15*F6</f>
         <v>8.0499999999999989</v>
       </c>
       <c r="C6" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D6+0.45*E6+0.05*F6</f>
         <v>8.2099999999999991</v>
       </c>
       <c r="D6" s="4">
@@ -1361,11 +1361,11 @@
         <v>37</v>
       </c>
       <c r="M6" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P6+0.8*Q6</f>
         <v>8.4</v>
       </c>
       <c r="N6" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q6+0.3*P6+0.2*O6</f>
         <v>9</v>
       </c>
       <c r="O6" s="17">
@@ -1383,11 +1383,11 @@
         <v>63</v>
       </c>
       <c r="B7" s="31">
-        <f t="shared" si="0"/>
+        <f>0.6*D7+0.25*E7+0.15*F7</f>
         <v>7.9550000000000001</v>
       </c>
       <c r="C7" s="34">
-        <f t="shared" si="1"/>
+        <f>0.5*D7+0.45*E7+0.05*F7</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D7" s="5">
@@ -1400,7 +1400,7 @@
         <v>8.5</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="H7" s="60"/>
       <c r="I7" s="60"/>
@@ -1410,11 +1410,11 @@
         <v>35</v>
       </c>
       <c r="M7" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P7+0.8*Q7</f>
         <v>8.4</v>
       </c>
       <c r="N7" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q7+0.3*P7+0.2*O7</f>
         <v>8.8000000000000007</v>
       </c>
       <c r="O7" s="17">
@@ -1427,16 +1427,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="33">
-        <f t="shared" si="0"/>
+        <f>0.6*D8+0.25*E8+0.15*F8</f>
         <v>6.55</v>
       </c>
       <c r="C8" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D8+0.45*E8+0.05*F8</f>
         <v>6.0100000000000007</v>
       </c>
       <c r="D8" s="44">
@@ -1456,11 +1456,11 @@
         <v>46</v>
       </c>
       <c r="M8" s="14">
-        <f t="shared" si="2"/>
+        <f>0.2*P8+0.8*Q8</f>
         <v>8.4</v>
       </c>
       <c r="N8" s="14">
-        <f t="shared" si="3"/>
+        <f>0.5*Q8+0.3*P8+0.2*O8</f>
         <v>8.6</v>
       </c>
       <c r="O8" s="19">
@@ -1473,16 +1473,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="33">
-        <f t="shared" si="0"/>
+        <f>0.6*D9+0.25*E9+0.15*F9</f>
         <v>5.3100000000000005</v>
       </c>
       <c r="C9" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D9+0.45*E9+0.05*F9</f>
         <v>5.37</v>
       </c>
       <c r="D9" s="44">
@@ -1502,11 +1502,11 @@
         <v>32</v>
       </c>
       <c r="M9" s="23">
-        <f t="shared" si="2"/>
+        <f>0.2*P9+0.8*Q9</f>
         <v>8</v>
       </c>
       <c r="N9" s="23">
-        <f t="shared" si="3"/>
+        <f>0.5*Q9+0.3*P9+0.2*O9</f>
         <v>5.6</v>
       </c>
       <c r="O9" s="24">
@@ -1519,16 +1519,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="33">
-        <f t="shared" si="0"/>
+        <f>0.6*D10+0.25*E10+0.15*F10</f>
         <v>4.7300000000000004</v>
       </c>
       <c r="C10" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D10+0.45*E10+0.05*F10</f>
         <v>4.6300000000000008</v>
       </c>
       <c r="D10" s="44">
@@ -1548,11 +1548,11 @@
         <v>10</v>
       </c>
       <c r="M10" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P10+0.8*Q10</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="N10" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q10+0.3*P10+0.2*O10</f>
         <v>8.3000000000000007</v>
       </c>
       <c r="O10" s="17">
@@ -1565,16 +1565,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="33">
-        <f t="shared" si="0"/>
+        <f>0.6*D11+0.25*E11+0.15*F11</f>
         <v>4.17</v>
       </c>
       <c r="C11" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D11+0.45*E11+0.05*F11</f>
         <v>4.08</v>
       </c>
       <c r="D11" s="44">
@@ -1594,11 +1594,11 @@
         <v>16</v>
       </c>
       <c r="M11" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P11+0.8*Q11</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="N11" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q11+0.3*P11+0.2*O11</f>
         <v>8.3000000000000007</v>
       </c>
       <c r="O11" s="17">
@@ -1616,11 +1616,11 @@
         <v>60</v>
       </c>
       <c r="B12" s="35">
-        <f t="shared" si="0"/>
+        <f>0.6*D12+0.25*E12+0.15*F12</f>
         <v>7.87</v>
       </c>
       <c r="C12" s="35">
-        <f t="shared" si="1"/>
+        <f>0.5*D12+0.45*E12+0.05*F12</f>
         <v>7.94</v>
       </c>
       <c r="D12" s="43">
@@ -1633,7 +1633,7 @@
         <v>8</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="H12" s="61"/>
       <c r="I12" s="61"/>
@@ -1643,11 +1643,11 @@
         <v>39</v>
       </c>
       <c r="M12" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P12+0.8*Q12</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="N12" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q12+0.3*P12+0.2*O12</f>
         <v>7.9</v>
       </c>
       <c r="O12" s="17">
@@ -1665,11 +1665,11 @@
         <v>62</v>
       </c>
       <c r="B13" s="33">
-        <f t="shared" si="0"/>
+        <f>0.6*D13+0.25*E13+0.15*F13</f>
         <v>7.7600000000000007</v>
       </c>
       <c r="C13" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D13+0.45*E13+0.05*F13</f>
         <v>7.5700000000000012</v>
       </c>
       <c r="D13" s="44">
@@ -1682,7 +1682,7 @@
         <v>7.2</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -1692,11 +1692,11 @@
         <v>34</v>
       </c>
       <c r="M13" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P13+0.8*Q13</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="N13" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q13+0.3*P13+0.2*O13</f>
         <v>7.5</v>
       </c>
       <c r="O13" s="17">
@@ -1714,11 +1714,11 @@
         <v>75</v>
       </c>
       <c r="B14" s="34">
-        <f t="shared" si="0"/>
+        <f>0.6*D14+0.25*E14+0.15*F14</f>
         <v>6.55</v>
       </c>
       <c r="C14" s="34">
-        <f t="shared" si="1"/>
+        <f>0.5*D14+0.45*E14+0.05*F14</f>
         <v>6.3</v>
       </c>
       <c r="D14" s="45">
@@ -1731,7 +1731,7 @@
         <v>6.5</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="H14" s="60"/>
       <c r="I14" s="60"/>
@@ -1741,11 +1741,11 @@
         <v>21</v>
       </c>
       <c r="M14" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P14+0.8*Q14</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="N14" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q14+0.3*P14+0.2*O14</f>
         <v>6.7</v>
       </c>
       <c r="O14" s="17">
@@ -1763,11 +1763,11 @@
         <v>70</v>
       </c>
       <c r="B15" s="35">
-        <f t="shared" si="0"/>
+        <f>0.6*D15+0.25*E15+0.15*F15</f>
         <v>6.2449999999999992</v>
       </c>
       <c r="C15" s="35">
-        <f t="shared" si="1"/>
+        <f>0.5*D15+0.45*E15+0.05*F15</f>
         <v>6.2150000000000007</v>
       </c>
       <c r="D15" s="43">
@@ -1790,11 +1790,11 @@
         <v>28</v>
       </c>
       <c r="M15" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P15+0.8*Q15</f>
         <v>6.8000000000000007</v>
       </c>
       <c r="N15" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q15+0.3*P15+0.2*O15</f>
         <v>7.6</v>
       </c>
       <c r="O15" s="17">
@@ -1812,11 +1812,11 @@
         <v>69</v>
       </c>
       <c r="B16" s="30">
-        <f t="shared" si="0"/>
+        <f>0.6*D16+0.25*E16+0.15*F16</f>
         <v>6.1849999999999996</v>
       </c>
       <c r="C16" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D16+0.45*E16+0.05*F16</f>
         <v>5.9550000000000001</v>
       </c>
       <c r="D16" s="44">
@@ -1829,7 +1829,7 @@
         <v>6.4</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
@@ -1839,11 +1839,11 @@
         <v>25</v>
       </c>
       <c r="M16" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P16+0.8*Q16</f>
         <v>6.8000000000000007</v>
       </c>
       <c r="N16" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q16+0.3*P16+0.2*O16</f>
         <v>7.4</v>
       </c>
       <c r="O16" s="17">
@@ -1861,11 +1861,11 @@
         <v>64</v>
       </c>
       <c r="B17" s="31">
-        <f t="shared" si="0"/>
+        <f>0.6*D17+0.25*E17+0.15*F17</f>
         <v>6.129999999999999</v>
       </c>
       <c r="C17" s="34">
-        <f t="shared" si="1"/>
+        <f>0.5*D17+0.45*E17+0.05*F17</f>
         <v>5.95</v>
       </c>
       <c r="D17" s="45">
@@ -1888,11 +1888,11 @@
         <v>33</v>
       </c>
       <c r="M17" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P17+0.8*Q17</f>
         <v>6.8000000000000007</v>
       </c>
       <c r="N17" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q17+0.3*P17+0.2*O17</f>
         <v>6.2</v>
       </c>
       <c r="O17" s="17">
@@ -1910,11 +1910,11 @@
         <v>66</v>
       </c>
       <c r="B18" s="32">
-        <f t="shared" si="0"/>
+        <f>0.6*D18+0.25*E18+0.15*F18</f>
         <v>5.74</v>
       </c>
       <c r="C18" s="35">
-        <f t="shared" si="1"/>
+        <f>0.5*D18+0.45*E18+0.05*F18</f>
         <v>5.6899999999999995</v>
       </c>
       <c r="D18" s="3">
@@ -1937,11 +1937,11 @@
         <v>40</v>
       </c>
       <c r="M18" s="14">
-        <f t="shared" si="2"/>
+        <f>0.2*P18+0.8*Q18</f>
         <v>6.8000000000000007</v>
       </c>
       <c r="N18" s="14">
-        <f t="shared" si="3"/>
+        <f>0.5*Q18+0.3*P18+0.2*O18</f>
         <v>6.2</v>
       </c>
       <c r="O18" s="19">
@@ -1959,11 +1959,11 @@
         <v>73</v>
       </c>
       <c r="B19" s="30">
-        <f t="shared" si="0"/>
+        <f>0.6*D19+0.25*E19+0.15*F19</f>
         <v>4.59</v>
       </c>
       <c r="C19" s="33">
-        <f t="shared" si="1"/>
+        <f>0.5*D19+0.45*E19+0.05*F19</f>
         <v>4.5199999999999996</v>
       </c>
       <c r="D19" s="4">
@@ -1986,11 +1986,11 @@
         <v>19</v>
       </c>
       <c r="M19" s="23">
-        <f t="shared" si="2"/>
+        <f>0.2*P19+0.8*Q19</f>
         <v>6.4</v>
       </c>
       <c r="N19" s="23">
-        <f t="shared" si="3"/>
+        <f>0.5*Q19+0.3*P19+0.2*O19</f>
         <v>5.6</v>
       </c>
       <c r="O19" s="24">
@@ -2008,11 +2008,11 @@
         <v>74</v>
       </c>
       <c r="B20" s="31">
-        <f t="shared" si="0"/>
+        <f>0.6*D20+0.25*E20+0.15*F20</f>
         <v>4.4950000000000001</v>
       </c>
       <c r="C20" s="34">
-        <f t="shared" si="1"/>
+        <f>0.5*D20+0.45*E20+0.05*F20</f>
         <v>4.2650000000000006</v>
       </c>
       <c r="D20" s="5">
@@ -2035,11 +2035,11 @@
         <v>18</v>
       </c>
       <c r="M20" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P20+0.8*Q20</f>
         <v>6.2000000000000011</v>
       </c>
       <c r="N20" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q20+0.3*P20+0.2*O20</f>
         <v>6.2</v>
       </c>
       <c r="O20" s="17">
@@ -2069,11 +2069,11 @@
         <v>43</v>
       </c>
       <c r="M21" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P21+0.8*Q21</f>
         <v>6</v>
       </c>
       <c r="N21" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q21+0.3*P21+0.2*O21</f>
         <v>6.1</v>
       </c>
       <c r="O21" s="17">
@@ -2091,11 +2091,11 @@
         <v>20</v>
       </c>
       <c r="M22" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P22+0.8*Q22</f>
         <v>5.6000000000000005</v>
       </c>
       <c r="N22" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q22+0.3*P22+0.2*O22</f>
         <v>5.3</v>
       </c>
       <c r="O22" s="17">
@@ -2113,11 +2113,11 @@
         <v>36</v>
       </c>
       <c r="M23" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P23+0.8*Q23</f>
         <v>5.6000000000000005</v>
       </c>
       <c r="N23" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q23+0.3*P23+0.2*O23</f>
         <v>4.5</v>
       </c>
       <c r="O23" s="17">
@@ -2135,11 +2135,11 @@
         <v>45</v>
       </c>
       <c r="M24" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P24+0.8*Q24</f>
         <v>5.6000000000000005</v>
       </c>
       <c r="N24" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q24+0.3*P24+0.2*O24</f>
         <v>4.3</v>
       </c>
       <c r="O24" s="17">
@@ -2157,11 +2157,11 @@
         <v>41</v>
       </c>
       <c r="M25" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P25+0.8*Q25</f>
         <v>5.4</v>
       </c>
       <c r="N25" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q25+0.3*P25+0.2*O25</f>
         <v>5.3999999999999995</v>
       </c>
       <c r="O25" s="17">
@@ -2179,11 +2179,11 @@
         <v>42</v>
       </c>
       <c r="M26" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P26+0.8*Q26</f>
         <v>5.2</v>
       </c>
       <c r="N26" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q26+0.3*P26+0.2*O26</f>
         <v>6.2</v>
       </c>
       <c r="O26" s="17">
@@ -2201,11 +2201,11 @@
         <v>44</v>
       </c>
       <c r="M27" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P27+0.8*Q27</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="N27" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q27+0.3*P27+0.2*O27</f>
         <v>5.7</v>
       </c>
       <c r="O27" s="17">
@@ -2223,11 +2223,11 @@
         <v>27</v>
       </c>
       <c r="M28" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P28+0.8*Q28</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="N28" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q28+0.3*P28+0.2*O28</f>
         <v>5.5</v>
       </c>
       <c r="O28" s="17">
@@ -2245,11 +2245,11 @@
         <v>7</v>
       </c>
       <c r="M29" s="14">
-        <f t="shared" si="2"/>
+        <f>0.2*P29+0.8*Q29</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="N29" s="14">
-        <f t="shared" si="3"/>
+        <f>0.5*Q29+0.3*P29+0.2*O29</f>
         <v>5.3</v>
       </c>
       <c r="O29" s="19">
@@ -2267,11 +2267,11 @@
         <v>17</v>
       </c>
       <c r="M30" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P30+0.8*Q30</f>
         <v>4</v>
       </c>
       <c r="N30" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q30+0.3*P30+0.2*O30</f>
         <v>3.3</v>
       </c>
       <c r="O30" s="17">
@@ -2289,11 +2289,11 @@
         <v>8</v>
       </c>
       <c r="M31" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P31+0.8*Q31</f>
         <v>4</v>
       </c>
       <c r="N31" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q31+0.3*P31+0.2*O31</f>
         <v>2.9</v>
       </c>
       <c r="O31" s="17">
@@ -2311,11 +2311,11 @@
         <v>15</v>
       </c>
       <c r="M32" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P32+0.8*Q32</f>
         <v>3.8000000000000003</v>
       </c>
       <c r="N32" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q32+0.3*P32+0.2*O32</f>
         <v>4.3</v>
       </c>
       <c r="O32" s="17">
@@ -2333,11 +2333,11 @@
         <v>26</v>
       </c>
       <c r="M33" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P33+0.8*Q33</f>
         <v>3.8000000000000003</v>
       </c>
       <c r="N33" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q33+0.3*P33+0.2*O33</f>
         <v>4.3</v>
       </c>
       <c r="O33" s="17">
@@ -2355,11 +2355,11 @@
         <v>13</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P34+0.8*Q34</f>
         <v>3.8000000000000003</v>
       </c>
       <c r="N34" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q34+0.3*P34+0.2*O34</f>
         <v>3.9</v>
       </c>
       <c r="O34" s="17">
@@ -2377,11 +2377,11 @@
         <v>12</v>
       </c>
       <c r="M35" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P35+0.8*Q35</f>
         <v>3.2</v>
       </c>
       <c r="N35" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q35+0.3*P35+0.2*O35</f>
         <v>3.6</v>
       </c>
       <c r="O35" s="17">
@@ -2399,11 +2399,11 @@
         <v>9</v>
       </c>
       <c r="M36" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P36+0.8*Q36</f>
         <v>3.2</v>
       </c>
       <c r="N36" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q36+0.3*P36+0.2*O36</f>
         <v>3.2</v>
       </c>
       <c r="O36" s="17">
@@ -2421,11 +2421,11 @@
         <v>23</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P37+0.8*Q37</f>
         <v>3.2</v>
       </c>
       <c r="N37" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q37+0.3*P37+0.2*O37</f>
         <v>3.2</v>
       </c>
       <c r="O37" s="17">
@@ -2443,11 +2443,11 @@
         <v>24</v>
       </c>
       <c r="M38" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P38+0.8*Q38</f>
         <v>3.2</v>
       </c>
       <c r="N38" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q38+0.3*P38+0.2*O38</f>
         <v>3.2</v>
       </c>
       <c r="O38" s="17">
@@ -2465,11 +2465,11 @@
         <v>47</v>
       </c>
       <c r="M39" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P39+0.8*Q39</f>
         <v>3.2</v>
       </c>
       <c r="N39" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q39+0.3*P39+0.2*O39</f>
         <v>3</v>
       </c>
       <c r="O39" s="17">
@@ -2487,11 +2487,11 @@
         <v>14</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" si="2"/>
+        <f>0.2*P40+0.8*Q40</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="N40" s="16">
-        <f t="shared" si="3"/>
+        <f>0.5*Q40+0.3*P40+0.2*O40</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="O40" s="17">
@@ -2509,11 +2509,11 @@
         <v>31</v>
       </c>
       <c r="M41" s="14">
-        <f t="shared" si="2"/>
+        <f>0.2*P41+0.8*Q41</f>
         <v>1.6</v>
       </c>
       <c r="N41" s="14">
-        <f t="shared" si="3"/>
+        <f>0.5*Q41+0.3*P41+0.2*O41</f>
         <v>1.8</v>
       </c>
       <c r="O41" s="19">

</xml_diff>